<commit_message>
PCB proj files initial commit
</commit_message>
<xml_diff>
--- a/docs/calculations.xlsx
+++ b/docs/calculations.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\clock\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\nixie-clock\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21705" windowHeight="12960"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21705" windowHeight="12960" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Power" sheetId="1" r:id="rId1"/>
+    <sheet name="Pins" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="33">
   <si>
     <t>Vsupply</t>
   </si>
@@ -54,14 +55,98 @@
   </si>
   <si>
     <t>mW</t>
+  </si>
+  <si>
+    <t>Vinput</t>
+  </si>
+  <si>
+    <t>Itube</t>
+  </si>
+  <si>
+    <t>Ptotal</t>
+  </si>
+  <si>
+    <t>Target 4W output power.</t>
+  </si>
+  <si>
+    <t>Efficiency</t>
+  </si>
+  <si>
+    <t>Pin</t>
+  </si>
+  <si>
+    <t>Iin</t>
+  </si>
+  <si>
+    <t>Vout</t>
+  </si>
+  <si>
+    <t>Vpri</t>
+  </si>
+  <si>
+    <t>duty</t>
+  </si>
+  <si>
+    <t>Turns,sec</t>
+  </si>
+  <si>
+    <t>Turns,pri</t>
+  </si>
+  <si>
+    <t>L, sec</t>
+  </si>
+  <si>
+    <t>L,pri</t>
+  </si>
+  <si>
+    <t>uH</t>
+  </si>
+  <si>
+    <t>kHz</t>
+  </si>
+  <si>
+    <t>f,typ</t>
+  </si>
+  <si>
+    <t>GPIO</t>
+  </si>
+  <si>
+    <t>Nixie Tubes</t>
+  </si>
+  <si>
+    <t>ADC</t>
+  </si>
+  <si>
+    <t>Buttons</t>
+  </si>
+  <si>
+    <t>Brightness Setting</t>
+  </si>
+  <si>
+    <t>HV PWM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -86,14 +171,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -106,6 +196,49 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>86384</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>67106</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7058025" y="1552575"/>
+          <a:ext cx="4725059" cy="3086531"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -371,38 +504,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2">
         <f>B1-B3</f>
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -413,7 +549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -424,7 +560,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -436,16 +572,258 @@
         <v>5</v>
       </c>
     </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <f>B5*B2</f>
+        <v>263.45454545454544</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12">
+        <v>180</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14">
+        <f>B12*B13</f>
+        <v>360</v>
+      </c>
+      <c r="C14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15">
+        <f>B14*6</f>
+        <v>2160</v>
+      </c>
+      <c r="C15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18">
+        <f>4000/B17</f>
+        <v>8000</v>
+      </c>
+      <c r="C18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19">
+        <f>B18/B11</f>
+        <v>1600</v>
+      </c>
+      <c r="C19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23">
+        <v>100</v>
+      </c>
+      <c r="C23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="3">
+        <f>B23*(B21*B21/(B22*B22))</f>
+        <v>0.69444444444444442</v>
+      </c>
+      <c r="C24" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26">
+        <f>B11</f>
+        <v>5</v>
+      </c>
+      <c r="C26" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" s="2">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28">
+        <f>B26*B22*B27/(1-B27)</f>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B30">
+        <v>100</v>
+      </c>
+      <c r="C30" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:C12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3">
+        <f>6*4</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="B6">
-        <f>B5*B2</f>
-        <v>244.36363636363637</v>
-      </c>
-      <c r="C6" t="s">
-        <v>9</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <f>SUM(B3:B11)</f>
+        <v>28</v>
+      </c>
+      <c r="C12">
+        <f>SUM(C3:C11)</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>